<commit_message>
refactoring into an rmd file. additional species data
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MMAB3\Documents\RStudio Projects\Plant Nutrition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BAC6AE8-AB8E-4385-ADB8-5846C348CD06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{464EA2DE-3E9B-42DA-8AB6-24920F53D2A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6DF183B6-C7A5-4299-88F5-06F25E78E8A8}"/>
+    <workbookView xWindow="13845" yWindow="525" windowWidth="12540" windowHeight="14340" xr2:uid="{6DF183B6-C7A5-4299-88F5-06F25E78E8A8}"/>
   </bookViews>
   <sheets>
     <sheet name="RFriendly" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="23">
   <si>
     <t>Species</t>
   </si>
@@ -98,6 +98,12 @@
   </si>
   <si>
     <t>Asclepiastuberosa</t>
+  </si>
+  <si>
+    <t>Amorpha</t>
+  </si>
+  <si>
+    <t>Baptisia</t>
   </si>
 </sst>
 </file>
@@ -506,23 +512,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0C02CD2-F61D-4638-82A2-24C13D55C41E}">
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I214"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A160" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E210" sqref="E210"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" customWidth="1"/>
-    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -551,7 +557,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -581,7 +587,7 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -611,7 +617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -641,7 +647,7 @@
         <v>0.33333333333333337</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -671,7 +677,7 @@
         <v>1.4999999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -701,7 +707,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -731,7 +737,7 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -761,7 +767,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -791,7 +797,7 @@
         <v>0.44444444444444448</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -821,7 +827,7 @@
         <v>0.4285714285714286</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -851,7 +857,7 @@
         <v>0.4285714285714286</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -881,7 +887,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -911,7 +917,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -932,7 +938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -953,7 +959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -974,7 +980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -995,7 +1001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1016,7 +1022,7 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1037,7 +1043,7 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -1058,7 +1064,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -1079,7 +1085,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -1100,7 +1106,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -1121,7 +1127,7 @@
         <v>3.4999999999999996</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -1142,7 +1148,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -1163,7 +1169,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -1184,7 +1190,7 @@
         <v>5.9999999999999991</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -1207,7 +1213,7 @@
         <v>3.666666666666667</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>20</v>
       </c>
@@ -1234,7 +1240,7 @@
         <v>2.3333333333333335</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>20</v>
       </c>
@@ -1261,7 +1267,7 @@
         <v>1.7777777777777779</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -1289,7 +1295,7 @@
         <v>1.8888888888888888</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>20</v>
       </c>
@@ -1317,7 +1323,7 @@
         <v>1.6666666666666665</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>20</v>
       </c>
@@ -1345,7 +1351,7 @@
         <v>1.3333333333333333</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>20</v>
       </c>
@@ -1373,7 +1379,7 @@
         <v>1.5714285714285716</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -1401,7 +1407,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>20</v>
       </c>
@@ -1429,7 +1435,7 @@
         <v>1.375</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>20</v>
       </c>
@@ -1457,7 +1463,7 @@
         <v>1.1111111111111112</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>20</v>
       </c>
@@ -1485,7 +1491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>20</v>
       </c>
@@ -1513,7 +1519,7 @@
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>20</v>
       </c>
@@ -1541,19 +1547,2979 @@
         <v>0.77777777777777768</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-      <c r="H40" s="5"/>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>21</v>
+      </c>
+      <c r="B40" t="s">
+        <v>4</v>
+      </c>
+      <c r="E40">
+        <v>0.5</v>
+      </c>
+      <c r="F40">
+        <v>0.5</v>
+      </c>
+      <c r="G40">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="H40">
+        <v>0.19500000000000001</v>
+      </c>
       <c r="I40" s="5"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5"/>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" t="s">
+        <v>4</v>
+      </c>
+      <c r="E41">
+        <v>0.9</v>
+      </c>
+      <c r="F41">
+        <v>0.4</v>
+      </c>
+      <c r="G41">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="H41">
+        <v>0.09</v>
+      </c>
       <c r="I41" s="5"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>21</v>
+      </c>
+      <c r="B42" t="s">
+        <v>4</v>
+      </c>
+      <c r="E42">
+        <v>0.5</v>
+      </c>
+      <c r="F42">
+        <v>0.5</v>
+      </c>
+      <c r="G42">
+        <v>0.06</v>
+      </c>
+      <c r="H42">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>21</v>
+      </c>
+      <c r="B43" t="s">
+        <v>4</v>
+      </c>
+      <c r="E43">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F43">
+        <v>0.5</v>
+      </c>
+      <c r="G43">
+        <v>0.155</v>
+      </c>
+      <c r="H43">
+        <v>0.155</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>21</v>
+      </c>
+      <c r="B44" t="s">
+        <v>4</v>
+      </c>
+      <c r="E44">
+        <v>0.4</v>
+      </c>
+      <c r="F44">
+        <v>0.3</v>
+      </c>
+      <c r="G44">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="H44">
+        <v>6.5000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>21</v>
+      </c>
+      <c r="B45" t="s">
+        <v>4</v>
+      </c>
+      <c r="E45">
+        <v>0.5</v>
+      </c>
+      <c r="F45">
+        <v>0.5</v>
+      </c>
+      <c r="G45">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="H45">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>21</v>
+      </c>
+      <c r="B46" t="s">
+        <v>4</v>
+      </c>
+      <c r="E46">
+        <v>0.4</v>
+      </c>
+      <c r="F46">
+        <v>0.3</v>
+      </c>
+      <c r="G46">
+        <v>0.05</v>
+      </c>
+      <c r="H46">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>21</v>
+      </c>
+      <c r="B47" t="s">
+        <v>4</v>
+      </c>
+      <c r="E47">
+        <v>1.5</v>
+      </c>
+      <c r="F47">
+        <v>0.9</v>
+      </c>
+      <c r="G47">
+        <v>0.17</v>
+      </c>
+      <c r="H47">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>21</v>
+      </c>
+      <c r="B48" t="s">
+        <v>4</v>
+      </c>
+      <c r="E48">
+        <v>0.3</v>
+      </c>
+      <c r="F48">
+        <v>0.2</v>
+      </c>
+      <c r="G48">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H48">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>21</v>
+      </c>
+      <c r="B49" t="s">
+        <v>4</v>
+      </c>
+      <c r="E49">
+        <v>0.7</v>
+      </c>
+      <c r="F49">
+        <v>0.6</v>
+      </c>
+      <c r="G49">
+        <v>0.13</v>
+      </c>
+      <c r="H49">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>21</v>
+      </c>
+      <c r="B50" t="s">
+        <v>4</v>
+      </c>
+      <c r="E50">
+        <v>0.4</v>
+      </c>
+      <c r="F50">
+        <v>0.5</v>
+      </c>
+      <c r="G50">
+        <v>0.5</v>
+      </c>
+      <c r="H50">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>21</v>
+      </c>
+      <c r="B51" t="s">
+        <v>4</v>
+      </c>
+      <c r="E51">
+        <v>0.4</v>
+      </c>
+      <c r="F51">
+        <v>0.3</v>
+      </c>
+      <c r="G51">
+        <v>0.45</v>
+      </c>
+      <c r="H51">
+        <v>8.5000000000000006E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>21</v>
+      </c>
+      <c r="B52" t="s">
+        <v>4</v>
+      </c>
+      <c r="E52">
+        <v>0.7</v>
+      </c>
+      <c r="F52">
+        <v>0.4</v>
+      </c>
+      <c r="G52">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="H52">
+        <v>9.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>21</v>
+      </c>
+      <c r="B53" t="s">
+        <v>4</v>
+      </c>
+      <c r="E53">
+        <v>0.1</v>
+      </c>
+      <c r="F53">
+        <v>0.1</v>
+      </c>
+      <c r="G53">
+        <v>0.02</v>
+      </c>
+      <c r="H53">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>21</v>
+      </c>
+      <c r="B54" t="s">
+        <v>4</v>
+      </c>
+      <c r="E54">
+        <v>0.3</v>
+      </c>
+      <c r="F54">
+        <v>0.2</v>
+      </c>
+      <c r="G54">
+        <v>0.05</v>
+      </c>
+      <c r="H54">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>21</v>
+      </c>
+      <c r="B55" t="s">
+        <v>4</v>
+      </c>
+      <c r="E55">
+        <v>0.8</v>
+      </c>
+      <c r="F55">
+        <v>0.6</v>
+      </c>
+      <c r="G55">
+        <v>0.1</v>
+      </c>
+      <c r="H55">
+        <v>0.155</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>21</v>
+      </c>
+      <c r="B56" t="s">
+        <v>4</v>
+      </c>
+      <c r="E56">
+        <v>0.6</v>
+      </c>
+      <c r="F56">
+        <v>0.4</v>
+      </c>
+      <c r="G56">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="H56">
+        <v>9.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>21</v>
+      </c>
+      <c r="B57" t="s">
+        <v>4</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57">
+        <v>0.8</v>
+      </c>
+      <c r="G57">
+        <v>0.11</v>
+      </c>
+      <c r="H57">
+        <v>0.14499999999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>21</v>
+      </c>
+      <c r="B58" t="s">
+        <v>4</v>
+      </c>
+      <c r="E58">
+        <v>0.7</v>
+      </c>
+      <c r="F58">
+        <v>0.5</v>
+      </c>
+      <c r="G58">
+        <v>0.12</v>
+      </c>
+      <c r="H58">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>21</v>
+      </c>
+      <c r="B59" t="s">
+        <v>4</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+      <c r="F59">
+        <v>0.4</v>
+      </c>
+      <c r="G59">
+        <v>0.12</v>
+      </c>
+      <c r="H59">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>21</v>
+      </c>
+      <c r="B60" t="s">
+        <v>4</v>
+      </c>
+      <c r="E60">
+        <v>0.6</v>
+      </c>
+      <c r="F60">
+        <v>0.8</v>
+      </c>
+      <c r="G60">
+        <v>0.05</v>
+      </c>
+      <c r="H60">
+        <v>9.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>21</v>
+      </c>
+      <c r="B61" t="s">
+        <v>4</v>
+      </c>
+      <c r="E61">
+        <v>0.8</v>
+      </c>
+      <c r="F61">
+        <v>0.8</v>
+      </c>
+      <c r="G61">
+        <v>0.11</v>
+      </c>
+      <c r="H61">
+        <v>0.16500000000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>21</v>
+      </c>
+      <c r="B62" t="s">
+        <v>4</v>
+      </c>
+      <c r="E62">
+        <v>0.6</v>
+      </c>
+      <c r="F62">
+        <v>0.4</v>
+      </c>
+      <c r="G62">
+        <v>0.95</v>
+      </c>
+      <c r="H62">
+        <v>8.5000000000000006E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>21</v>
+      </c>
+      <c r="B63" t="s">
+        <v>4</v>
+      </c>
+      <c r="E63">
+        <v>0.7</v>
+      </c>
+      <c r="F63">
+        <v>0.6</v>
+      </c>
+      <c r="G63">
+        <v>0.1</v>
+      </c>
+      <c r="H63">
+        <v>0.155</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>21</v>
+      </c>
+      <c r="B64" t="s">
+        <v>4</v>
+      </c>
+      <c r="E64">
+        <v>0.2</v>
+      </c>
+      <c r="F64">
+        <v>0.2</v>
+      </c>
+      <c r="G64">
+        <v>0.02</v>
+      </c>
+      <c r="H64">
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>21</v>
+      </c>
+      <c r="B65" t="s">
+        <v>4</v>
+      </c>
+      <c r="E65">
+        <v>0.8</v>
+      </c>
+      <c r="F65">
+        <v>0.4</v>
+      </c>
+      <c r="G65">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="H65">
+        <v>0.115</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>21</v>
+      </c>
+      <c r="B66" t="s">
+        <v>4</v>
+      </c>
+      <c r="E66">
+        <v>0.2</v>
+      </c>
+      <c r="F66">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="G66">
+        <v>0.05</v>
+      </c>
+      <c r="H66">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>21</v>
+      </c>
+      <c r="B67" t="s">
+        <v>4</v>
+      </c>
+      <c r="E67">
+        <v>0.08</v>
+      </c>
+      <c r="F67">
+        <v>0.1</v>
+      </c>
+      <c r="G67">
+        <v>0.02</v>
+      </c>
+      <c r="H67">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>21</v>
+      </c>
+      <c r="B68" t="s">
+        <v>4</v>
+      </c>
+      <c r="E68">
+        <v>0.4</v>
+      </c>
+      <c r="F68">
+        <v>0.2</v>
+      </c>
+      <c r="G68">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="H68">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>21</v>
+      </c>
+      <c r="B69" t="s">
+        <v>4</v>
+      </c>
+      <c r="E69">
+        <v>0.7</v>
+      </c>
+      <c r="F69">
+        <v>0.6</v>
+      </c>
+      <c r="G69">
+        <v>0.115</v>
+      </c>
+      <c r="H69">
+        <v>0.185</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>21</v>
+      </c>
+      <c r="B70" t="s">
+        <v>4</v>
+      </c>
+      <c r="E70">
+        <v>0.4</v>
+      </c>
+      <c r="F70">
+        <v>0.25</v>
+      </c>
+      <c r="G70">
+        <v>0.75</v>
+      </c>
+      <c r="H70">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>21</v>
+      </c>
+      <c r="B71" t="s">
+        <v>4</v>
+      </c>
+      <c r="E71">
+        <v>0.5</v>
+      </c>
+      <c r="F71">
+        <v>0.3</v>
+      </c>
+      <c r="G71">
+        <v>0.06</v>
+      </c>
+      <c r="H71">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>21</v>
+      </c>
+      <c r="B72" t="s">
+        <v>4</v>
+      </c>
+      <c r="E72">
+        <v>1.3</v>
+      </c>
+      <c r="F72">
+        <v>0.6</v>
+      </c>
+      <c r="G72">
+        <v>0.17</v>
+      </c>
+      <c r="H72">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>21</v>
+      </c>
+      <c r="B73" t="s">
+        <v>4</v>
+      </c>
+      <c r="E73">
+        <v>1</v>
+      </c>
+      <c r="F73">
+        <v>0.5</v>
+      </c>
+      <c r="G73">
+        <v>0.125</v>
+      </c>
+      <c r="H73">
+        <v>0.17499999999999999</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>21</v>
+      </c>
+      <c r="B74" t="s">
+        <v>4</v>
+      </c>
+      <c r="E74">
+        <v>1</v>
+      </c>
+      <c r="F74">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G74">
+        <v>0.15</v>
+      </c>
+      <c r="H74">
+        <v>0.215</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>21</v>
+      </c>
+      <c r="B75" t="s">
+        <v>4</v>
+      </c>
+      <c r="E75">
+        <v>0.6</v>
+      </c>
+      <c r="F75">
+        <v>0.2</v>
+      </c>
+      <c r="G75">
+        <v>0.06</v>
+      </c>
+      <c r="H75">
+        <v>6.5000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>21</v>
+      </c>
+      <c r="B76" t="s">
+        <v>4</v>
+      </c>
+      <c r="E76">
+        <v>0.7</v>
+      </c>
+      <c r="F76">
+        <v>0.7</v>
+      </c>
+      <c r="G76">
+        <v>0.09</v>
+      </c>
+      <c r="H76">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>21</v>
+      </c>
+      <c r="B77" t="s">
+        <v>4</v>
+      </c>
+      <c r="E77">
+        <v>0.2</v>
+      </c>
+      <c r="F77">
+        <v>0.3</v>
+      </c>
+      <c r="G77">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H77">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>21</v>
+      </c>
+      <c r="B78" t="s">
+        <v>4</v>
+      </c>
+      <c r="E78">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F78">
+        <v>0.5</v>
+      </c>
+      <c r="G78">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H78">
+        <v>0.155</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>21</v>
+      </c>
+      <c r="B79" t="s">
+        <v>4</v>
+      </c>
+      <c r="E79">
+        <v>0.4</v>
+      </c>
+      <c r="F79">
+        <v>0.2</v>
+      </c>
+      <c r="G79">
+        <v>5.5E-2</v>
+      </c>
+      <c r="H79">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>21</v>
+      </c>
+      <c r="B80" t="s">
+        <v>4</v>
+      </c>
+      <c r="E80">
+        <v>0.8</v>
+      </c>
+      <c r="F80">
+        <v>0.7</v>
+      </c>
+      <c r="G80">
+        <v>0.125</v>
+      </c>
+      <c r="H80">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>21</v>
+      </c>
+      <c r="B81" t="s">
+        <v>4</v>
+      </c>
+      <c r="E81">
+        <v>0.2</v>
+      </c>
+      <c r="F81">
+        <v>0.2</v>
+      </c>
+      <c r="G81">
+        <v>0.02</v>
+      </c>
+      <c r="H81">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>21</v>
+      </c>
+      <c r="B82" t="s">
+        <v>4</v>
+      </c>
+      <c r="E82">
+        <v>0.6</v>
+      </c>
+      <c r="F82">
+        <v>0.9</v>
+      </c>
+      <c r="G82">
+        <v>0.11</v>
+      </c>
+      <c r="H82">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>21</v>
+      </c>
+      <c r="B83" t="s">
+        <v>4</v>
+      </c>
+      <c r="E83">
+        <v>0.8</v>
+      </c>
+      <c r="F83">
+        <v>0.5</v>
+      </c>
+      <c r="G83">
+        <v>0.11</v>
+      </c>
+      <c r="H83">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>21</v>
+      </c>
+      <c r="B84" t="s">
+        <v>4</v>
+      </c>
+      <c r="E84">
+        <v>0.1</v>
+      </c>
+      <c r="F84">
+        <v>0.06</v>
+      </c>
+      <c r="G84">
+        <v>0.02</v>
+      </c>
+      <c r="H84">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>21</v>
+      </c>
+      <c r="B85" t="s">
+        <v>3</v>
+      </c>
+      <c r="E85">
+        <v>0.5</v>
+      </c>
+      <c r="F85">
+        <v>0.2</v>
+      </c>
+      <c r="G85">
+        <v>0.1</v>
+      </c>
+      <c r="H85">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>21</v>
+      </c>
+      <c r="B86" t="s">
+        <v>3</v>
+      </c>
+      <c r="E86">
+        <v>0.6</v>
+      </c>
+      <c r="F86">
+        <v>0.3</v>
+      </c>
+      <c r="G86">
+        <v>0.11</v>
+      </c>
+      <c r="H86">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>21</v>
+      </c>
+      <c r="B87" t="s">
+        <v>3</v>
+      </c>
+      <c r="E87">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F87">
+        <v>0.6</v>
+      </c>
+      <c r="G87">
+        <v>0.17</v>
+      </c>
+      <c r="H87">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>21</v>
+      </c>
+      <c r="B88" t="s">
+        <v>3</v>
+      </c>
+      <c r="E88">
+        <v>0.6</v>
+      </c>
+      <c r="F88">
+        <v>0.4</v>
+      </c>
+      <c r="G88">
+        <v>0.13</v>
+      </c>
+      <c r="H88">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>21</v>
+      </c>
+      <c r="B89" t="s">
+        <v>3</v>
+      </c>
+      <c r="E89">
+        <v>0.2</v>
+      </c>
+      <c r="F89">
+        <v>0.1</v>
+      </c>
+      <c r="G89">
+        <v>0.04</v>
+      </c>
+      <c r="H89">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>21</v>
+      </c>
+      <c r="B90" t="s">
+        <v>3</v>
+      </c>
+      <c r="E90">
+        <v>0.8</v>
+      </c>
+      <c r="F90">
+        <v>0.7</v>
+      </c>
+      <c r="G90">
+        <v>0.11</v>
+      </c>
+      <c r="H90">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>21</v>
+      </c>
+      <c r="B91" t="s">
+        <v>3</v>
+      </c>
+      <c r="E91">
+        <v>0.3</v>
+      </c>
+      <c r="F91">
+        <v>0.3</v>
+      </c>
+      <c r="G91">
+        <v>0.05</v>
+      </c>
+      <c r="H91">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>21</v>
+      </c>
+      <c r="B92" t="s">
+        <v>3</v>
+      </c>
+      <c r="E92">
+        <v>0.4</v>
+      </c>
+      <c r="F92">
+        <v>0.3</v>
+      </c>
+      <c r="G92">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="H92">
+        <v>8.5000000000000006E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>21</v>
+      </c>
+      <c r="B93" t="s">
+        <v>3</v>
+      </c>
+      <c r="E93">
+        <v>1.3</v>
+      </c>
+      <c r="F93">
+        <v>0.4</v>
+      </c>
+      <c r="G93">
+        <v>0.23</v>
+      </c>
+      <c r="H93">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>21</v>
+      </c>
+      <c r="B94" t="s">
+        <v>3</v>
+      </c>
+      <c r="E94">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F94">
+        <v>0.7</v>
+      </c>
+      <c r="G94">
+        <v>0.18</v>
+      </c>
+      <c r="H94">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>21</v>
+      </c>
+      <c r="B95" t="s">
+        <v>3</v>
+      </c>
+      <c r="E95">
+        <v>1.3</v>
+      </c>
+      <c r="F95">
+        <v>0.7</v>
+      </c>
+      <c r="G95">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="H95">
+        <v>0.17499999999999999</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>21</v>
+      </c>
+      <c r="B96" t="s">
+        <v>3</v>
+      </c>
+      <c r="E96">
+        <v>0.6</v>
+      </c>
+      <c r="F96">
+        <v>0.6</v>
+      </c>
+      <c r="G96">
+        <v>0.08</v>
+      </c>
+      <c r="H96">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>21</v>
+      </c>
+      <c r="B97" t="s">
+        <v>3</v>
+      </c>
+      <c r="E97">
+        <v>0.6</v>
+      </c>
+      <c r="F97">
+        <v>0.2</v>
+      </c>
+      <c r="G97">
+        <v>0.12</v>
+      </c>
+      <c r="H97">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>21</v>
+      </c>
+      <c r="B98" t="s">
+        <v>3</v>
+      </c>
+      <c r="E98">
+        <v>1.3</v>
+      </c>
+      <c r="F98">
+        <v>0.8</v>
+      </c>
+      <c r="G98">
+        <v>0.19</v>
+      </c>
+      <c r="H98">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>21</v>
+      </c>
+      <c r="B99" t="s">
+        <v>3</v>
+      </c>
+      <c r="E99">
+        <v>0.3</v>
+      </c>
+      <c r="F99">
+        <v>0.2</v>
+      </c>
+      <c r="G99">
+        <v>0.02</v>
+      </c>
+      <c r="H99">
+        <v>6.5000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>21</v>
+      </c>
+      <c r="B100" t="s">
+        <v>3</v>
+      </c>
+      <c r="E100">
+        <v>1.4</v>
+      </c>
+      <c r="F100">
+        <v>0.6</v>
+      </c>
+      <c r="G100">
+        <v>0.21</v>
+      </c>
+      <c r="H100">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>21</v>
+      </c>
+      <c r="B101" t="s">
+        <v>3</v>
+      </c>
+      <c r="E101">
+        <v>0.7</v>
+      </c>
+      <c r="F101">
+        <v>0.2</v>
+      </c>
+      <c r="G101">
+        <v>0.08</v>
+      </c>
+      <c r="H101">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>21</v>
+      </c>
+      <c r="B102" t="s">
+        <v>3</v>
+      </c>
+      <c r="E102">
+        <v>0.5</v>
+      </c>
+      <c r="F102">
+        <v>0.2</v>
+      </c>
+      <c r="G102">
+        <v>0.08</v>
+      </c>
+      <c r="H102">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>21</v>
+      </c>
+      <c r="B103" t="s">
+        <v>3</v>
+      </c>
+      <c r="E103">
+        <v>0.3</v>
+      </c>
+      <c r="F103">
+        <v>0.2</v>
+      </c>
+      <c r="G103">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H103">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>21</v>
+      </c>
+      <c r="B104" t="s">
+        <v>3</v>
+      </c>
+      <c r="E104">
+        <v>1.2</v>
+      </c>
+      <c r="F104">
+        <v>0.5</v>
+      </c>
+      <c r="G104">
+        <v>0.215</v>
+      </c>
+      <c r="H104">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>21</v>
+      </c>
+      <c r="B105" t="s">
+        <v>3</v>
+      </c>
+      <c r="E105">
+        <v>0.5</v>
+      </c>
+      <c r="F105">
+        <v>0.5</v>
+      </c>
+      <c r="G105">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="H105">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>21</v>
+      </c>
+      <c r="B106" t="s">
+        <v>3</v>
+      </c>
+      <c r="E106">
+        <v>1.2</v>
+      </c>
+      <c r="F106">
+        <v>0.4</v>
+      </c>
+      <c r="G106">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H106">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>21</v>
+      </c>
+      <c r="B107" t="s">
+        <v>3</v>
+      </c>
+      <c r="E107">
+        <v>0.8</v>
+      </c>
+      <c r="F107">
+        <v>0.5</v>
+      </c>
+      <c r="G107">
+        <v>0.125</v>
+      </c>
+      <c r="H107">
+        <v>0.105</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>21</v>
+      </c>
+      <c r="B108" t="s">
+        <v>3</v>
+      </c>
+      <c r="E108">
+        <v>0.4</v>
+      </c>
+      <c r="F108">
+        <v>0.3</v>
+      </c>
+      <c r="G108">
+        <v>0.05</v>
+      </c>
+      <c r="H108">
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>21</v>
+      </c>
+      <c r="B109" t="s">
+        <v>3</v>
+      </c>
+      <c r="E109">
+        <v>0.6</v>
+      </c>
+      <c r="F109">
+        <v>0.3</v>
+      </c>
+      <c r="G109">
+        <v>0.1</v>
+      </c>
+      <c r="H109">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>21</v>
+      </c>
+      <c r="B110" t="s">
+        <v>3</v>
+      </c>
+      <c r="E110">
+        <v>0.4</v>
+      </c>
+      <c r="F110">
+        <v>0.2</v>
+      </c>
+      <c r="G110">
+        <v>0.08</v>
+      </c>
+      <c r="H110">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>21</v>
+      </c>
+      <c r="B111" t="s">
+        <v>3</v>
+      </c>
+      <c r="E111">
+        <v>0.3</v>
+      </c>
+      <c r="F111">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="G111">
+        <v>0.03</v>
+      </c>
+      <c r="H111">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>21</v>
+      </c>
+      <c r="B112" t="s">
+        <v>3</v>
+      </c>
+      <c r="E112">
+        <v>0.8</v>
+      </c>
+      <c r="F112">
+        <v>0.4</v>
+      </c>
+      <c r="G112">
+        <v>0.155</v>
+      </c>
+      <c r="H112">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>21</v>
+      </c>
+      <c r="B113" t="s">
+        <v>3</v>
+      </c>
+      <c r="E113">
+        <v>0.5</v>
+      </c>
+      <c r="F113">
+        <v>0.2</v>
+      </c>
+      <c r="G113">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="H113">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>21</v>
+      </c>
+      <c r="B114" t="s">
+        <v>3</v>
+      </c>
+      <c r="E114">
+        <v>0.4</v>
+      </c>
+      <c r="F114">
+        <v>0.1</v>
+      </c>
+      <c r="G114">
+        <v>0.4</v>
+      </c>
+      <c r="H114">
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>21</v>
+      </c>
+      <c r="B115" t="s">
+        <v>3</v>
+      </c>
+      <c r="E115">
+        <v>0.5</v>
+      </c>
+      <c r="F115">
+        <v>0.1</v>
+      </c>
+      <c r="G115">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="H115">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>21</v>
+      </c>
+      <c r="B116" t="s">
+        <v>3</v>
+      </c>
+      <c r="E116">
+        <v>0.3</v>
+      </c>
+      <c r="F116">
+        <v>0.2</v>
+      </c>
+      <c r="G116">
+        <v>0.06</v>
+      </c>
+      <c r="H116">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>21</v>
+      </c>
+      <c r="B117" t="s">
+        <v>3</v>
+      </c>
+      <c r="E117">
+        <v>0.6</v>
+      </c>
+      <c r="F117">
+        <v>0.4</v>
+      </c>
+      <c r="G117">
+        <v>0.08</v>
+      </c>
+      <c r="H117">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>21</v>
+      </c>
+      <c r="B118" t="s">
+        <v>3</v>
+      </c>
+      <c r="E118">
+        <v>0.5</v>
+      </c>
+      <c r="F118">
+        <v>0.2</v>
+      </c>
+      <c r="G118">
+        <v>0.05</v>
+      </c>
+      <c r="H118">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>21</v>
+      </c>
+      <c r="B119" t="s">
+        <v>3</v>
+      </c>
+      <c r="E119">
+        <v>1.7</v>
+      </c>
+      <c r="F119">
+        <v>1</v>
+      </c>
+      <c r="G119">
+        <v>0.24</v>
+      </c>
+      <c r="H119">
+        <v>0.315</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>21</v>
+      </c>
+      <c r="B120" t="s">
+        <v>3</v>
+      </c>
+      <c r="E120">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F120">
+        <v>0.4</v>
+      </c>
+      <c r="G120">
+        <v>0.17</v>
+      </c>
+      <c r="H120">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>21</v>
+      </c>
+      <c r="B121" t="s">
+        <v>3</v>
+      </c>
+      <c r="E121">
+        <v>0.3</v>
+      </c>
+      <c r="F121">
+        <v>0.2</v>
+      </c>
+      <c r="G121">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="H121">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>21</v>
+      </c>
+      <c r="B122" t="s">
+        <v>3</v>
+      </c>
+      <c r="E122">
+        <v>0.5</v>
+      </c>
+      <c r="F122">
+        <v>0.3</v>
+      </c>
+      <c r="G122">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="H122">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>21</v>
+      </c>
+      <c r="B123" t="s">
+        <v>3</v>
+      </c>
+      <c r="E123">
+        <v>0.4</v>
+      </c>
+      <c r="F123">
+        <v>0.3</v>
+      </c>
+      <c r="G123">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="H123">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>21</v>
+      </c>
+      <c r="B124" t="s">
+        <v>3</v>
+      </c>
+      <c r="E124">
+        <v>0.5</v>
+      </c>
+      <c r="F124">
+        <v>0.3</v>
+      </c>
+      <c r="G124">
+        <v>0.08</v>
+      </c>
+      <c r="H124">
+        <v>5.5E-2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>21</v>
+      </c>
+      <c r="B125" t="s">
+        <v>3</v>
+      </c>
+      <c r="E125">
+        <v>0.5</v>
+      </c>
+      <c r="F125">
+        <v>0.1</v>
+      </c>
+      <c r="G125">
+        <v>0.09</v>
+      </c>
+      <c r="H125">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>21</v>
+      </c>
+      <c r="B126" t="s">
+        <v>3</v>
+      </c>
+      <c r="E126">
+        <v>0.4</v>
+      </c>
+      <c r="F126">
+        <v>0.2</v>
+      </c>
+      <c r="G126">
+        <v>0.06</v>
+      </c>
+      <c r="H126">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>21</v>
+      </c>
+      <c r="B127" t="s">
+        <v>3</v>
+      </c>
+      <c r="E127">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F127">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>22</v>
+      </c>
+      <c r="B128" t="s">
+        <v>3</v>
+      </c>
+      <c r="G128">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="H128">
+        <v>0.14499999999999999</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>22</v>
+      </c>
+      <c r="B129" t="s">
+        <v>3</v>
+      </c>
+      <c r="G129">
+        <v>0.21</v>
+      </c>
+      <c r="H129">
+        <v>0.17499999999999999</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>22</v>
+      </c>
+      <c r="B130" t="s">
+        <v>3</v>
+      </c>
+      <c r="G130">
+        <v>0.12</v>
+      </c>
+      <c r="H130">
+        <v>0.105</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>22</v>
+      </c>
+      <c r="B131" t="s">
+        <v>3</v>
+      </c>
+      <c r="G131">
+        <v>0.11</v>
+      </c>
+      <c r="H131">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>22</v>
+      </c>
+      <c r="B132" t="s">
+        <v>3</v>
+      </c>
+      <c r="G132">
+        <v>0.09</v>
+      </c>
+      <c r="H132">
+        <v>8.5000000000000006E-2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>22</v>
+      </c>
+      <c r="B133" t="s">
+        <v>3</v>
+      </c>
+      <c r="G133">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="H133">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>22</v>
+      </c>
+      <c r="B134" t="s">
+        <v>3</v>
+      </c>
+      <c r="G134">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="H134">
+        <v>0.185</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>22</v>
+      </c>
+      <c r="B135" t="s">
+        <v>3</v>
+      </c>
+      <c r="G135">
+        <v>0.15</v>
+      </c>
+      <c r="H135">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>22</v>
+      </c>
+      <c r="B136" t="s">
+        <v>3</v>
+      </c>
+      <c r="G136">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="H136">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>22</v>
+      </c>
+      <c r="B137" t="s">
+        <v>3</v>
+      </c>
+      <c r="G137">
+        <v>0.115</v>
+      </c>
+      <c r="H137">
+        <v>0.155</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>22</v>
+      </c>
+      <c r="B138" t="s">
+        <v>3</v>
+      </c>
+      <c r="G138">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="H138">
+        <v>0.17499999999999999</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>22</v>
+      </c>
+      <c r="B139" t="s">
+        <v>3</v>
+      </c>
+      <c r="G139">
+        <v>0.22</v>
+      </c>
+      <c r="H139">
+        <v>0.16500000000000001</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>22</v>
+      </c>
+      <c r="B140" t="s">
+        <v>3</v>
+      </c>
+      <c r="G140">
+        <v>0.23</v>
+      </c>
+      <c r="H140">
+        <v>0.215</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>22</v>
+      </c>
+      <c r="B141" t="s">
+        <v>3</v>
+      </c>
+      <c r="G141">
+        <v>0.17</v>
+      </c>
+      <c r="H141">
+        <v>0.16500000000000001</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>22</v>
+      </c>
+      <c r="B142" t="s">
+        <v>3</v>
+      </c>
+      <c r="G142">
+        <v>0.09</v>
+      </c>
+      <c r="H142">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>22</v>
+      </c>
+      <c r="B143" t="s">
+        <v>3</v>
+      </c>
+      <c r="G143">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="H143">
+        <v>0.155</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>22</v>
+      </c>
+      <c r="B144" t="s">
+        <v>3</v>
+      </c>
+      <c r="G144">
+        <v>0.115</v>
+      </c>
+      <c r="H144">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>22</v>
+      </c>
+      <c r="B145" t="s">
+        <v>3</v>
+      </c>
+      <c r="G145">
+        <v>0.2</v>
+      </c>
+      <c r="H145">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>22</v>
+      </c>
+      <c r="B146" t="s">
+        <v>3</v>
+      </c>
+      <c r="G146">
+        <v>0.215</v>
+      </c>
+      <c r="H146">
+        <v>0.22500000000000001</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>22</v>
+      </c>
+      <c r="B147" t="s">
+        <v>3</v>
+      </c>
+      <c r="G147">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="H147">
+        <v>0.14499999999999999</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>22</v>
+      </c>
+      <c r="B148" t="s">
+        <v>3</v>
+      </c>
+      <c r="G148">
+        <v>0.12</v>
+      </c>
+      <c r="H148">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>22</v>
+      </c>
+      <c r="B149" t="s">
+        <v>3</v>
+      </c>
+      <c r="G149">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="H149">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>22</v>
+      </c>
+      <c r="B150" t="s">
+        <v>3</v>
+      </c>
+      <c r="G150">
+        <v>0.32</v>
+      </c>
+      <c r="H150">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>22</v>
+      </c>
+      <c r="B151" t="s">
+        <v>3</v>
+      </c>
+      <c r="G151">
+        <v>0.15</v>
+      </c>
+      <c r="H151">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>22</v>
+      </c>
+      <c r="B152" t="s">
+        <v>3</v>
+      </c>
+      <c r="G152">
+        <v>0.12</v>
+      </c>
+      <c r="H152">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>22</v>
+      </c>
+      <c r="B153" t="s">
+        <v>3</v>
+      </c>
+      <c r="G153">
+        <v>0.4</v>
+      </c>
+      <c r="H153">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>22</v>
+      </c>
+      <c r="B154" t="s">
+        <v>3</v>
+      </c>
+      <c r="G154">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="H154">
+        <v>0.105</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>22</v>
+      </c>
+      <c r="B155" t="s">
+        <v>3</v>
+      </c>
+      <c r="G155">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="H155">
+        <v>0.22500000000000001</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
+        <v>22</v>
+      </c>
+      <c r="B156" t="s">
+        <v>3</v>
+      </c>
+      <c r="G156">
+        <v>0.155</v>
+      </c>
+      <c r="H156">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
+        <v>22</v>
+      </c>
+      <c r="B157" t="s">
+        <v>3</v>
+      </c>
+      <c r="G157">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="H157">
+        <v>5.5E-2</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
+        <v>22</v>
+      </c>
+      <c r="B158" t="s">
+        <v>3</v>
+      </c>
+      <c r="G158">
+        <v>0.17</v>
+      </c>
+      <c r="H158">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
+        <v>22</v>
+      </c>
+      <c r="B159" t="s">
+        <v>3</v>
+      </c>
+      <c r="G159">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="H159">
+        <v>0.14499999999999999</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
+        <v>22</v>
+      </c>
+      <c r="B160" t="s">
+        <v>3</v>
+      </c>
+      <c r="G160">
+        <v>0.21</v>
+      </c>
+      <c r="H160">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>22</v>
+      </c>
+      <c r="B161" t="s">
+        <v>3</v>
+      </c>
+      <c r="G161">
+        <v>0.34</v>
+      </c>
+      <c r="H161">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
+        <v>22</v>
+      </c>
+      <c r="B162" t="s">
+        <v>3</v>
+      </c>
+      <c r="G162">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H162">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>22</v>
+      </c>
+      <c r="B163" t="s">
+        <v>3</v>
+      </c>
+      <c r="G163">
+        <v>0.15</v>
+      </c>
+      <c r="H163">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>22</v>
+      </c>
+      <c r="B164" t="s">
+        <v>3</v>
+      </c>
+      <c r="G164">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="H164">
+        <v>0.105</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>22</v>
+      </c>
+      <c r="B165" t="s">
+        <v>3</v>
+      </c>
+      <c r="G165">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="H165">
+        <v>9.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
+        <v>22</v>
+      </c>
+      <c r="B166" t="s">
+        <v>3</v>
+      </c>
+      <c r="G166">
+        <v>0.17</v>
+      </c>
+      <c r="H166">
+        <v>0.115</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
+        <v>22</v>
+      </c>
+      <c r="B167" t="s">
+        <v>3</v>
+      </c>
+      <c r="G167">
+        <v>0.21</v>
+      </c>
+      <c r="H167">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
+        <v>22</v>
+      </c>
+      <c r="B168" t="s">
+        <v>3</v>
+      </c>
+      <c r="G168">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="H168">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
+        <v>22</v>
+      </c>
+      <c r="B169" t="s">
+        <v>3</v>
+      </c>
+      <c r="G169">
+        <v>0.31</v>
+      </c>
+      <c r="H169">
+        <v>0.22500000000000001</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>22</v>
+      </c>
+      <c r="B170" t="s">
+        <v>3</v>
+      </c>
+      <c r="G170">
+        <v>0.255</v>
+      </c>
+      <c r="H170">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A171" t="s">
+        <v>22</v>
+      </c>
+      <c r="B171" t="s">
+        <v>3</v>
+      </c>
+      <c r="G171">
+        <v>0.27</v>
+      </c>
+      <c r="H171">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
+        <v>22</v>
+      </c>
+      <c r="B172" t="s">
+        <v>3</v>
+      </c>
+      <c r="G172">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="H172">
+        <v>0.185</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A173" t="s">
+        <v>22</v>
+      </c>
+      <c r="B173" t="s">
+        <v>3</v>
+      </c>
+      <c r="G173">
+        <v>0.125</v>
+      </c>
+      <c r="H173">
+        <v>0.105</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
+        <v>22</v>
+      </c>
+      <c r="B174" t="s">
+        <v>4</v>
+      </c>
+      <c r="G174">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="H174">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A175" t="s">
+        <v>22</v>
+      </c>
+      <c r="B175" t="s">
+        <v>4</v>
+      </c>
+      <c r="G175">
+        <v>0.43</v>
+      </c>
+      <c r="H175">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
+        <v>22</v>
+      </c>
+      <c r="B176" t="s">
+        <v>4</v>
+      </c>
+      <c r="G176">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H176">
+        <v>0.30499999999999999</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A177" t="s">
+        <v>22</v>
+      </c>
+      <c r="B177" t="s">
+        <v>4</v>
+      </c>
+      <c r="G177">
+        <v>0.105</v>
+      </c>
+      <c r="H177">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A178" t="s">
+        <v>22</v>
+      </c>
+      <c r="B178" t="s">
+        <v>4</v>
+      </c>
+      <c r="G178">
+        <v>0.3</v>
+      </c>
+      <c r="H178">
+        <v>0.27500000000000002</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A179" t="s">
+        <v>22</v>
+      </c>
+      <c r="B179" t="s">
+        <v>4</v>
+      </c>
+      <c r="G179">
+        <v>0.2</v>
+      </c>
+      <c r="H179">
+        <v>0.20499999999999999</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
+        <v>22</v>
+      </c>
+      <c r="B180" t="s">
+        <v>4</v>
+      </c>
+      <c r="G180">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="H180">
+        <v>0.17499999999999999</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A181" t="s">
+        <v>22</v>
+      </c>
+      <c r="B181" t="s">
+        <v>4</v>
+      </c>
+      <c r="G181">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="H181">
+        <v>0.33500000000000002</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A182" t="s">
+        <v>22</v>
+      </c>
+      <c r="B182" t="s">
+        <v>4</v>
+      </c>
+      <c r="G182">
+        <v>0.38</v>
+      </c>
+      <c r="H182">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A183" t="s">
+        <v>22</v>
+      </c>
+      <c r="B183" t="s">
+        <v>4</v>
+      </c>
+      <c r="G183">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="H183">
+        <v>0.41499999999999998</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A184" t="s">
+        <v>22</v>
+      </c>
+      <c r="B184" t="s">
+        <v>4</v>
+      </c>
+      <c r="G184">
+        <v>0.26</v>
+      </c>
+      <c r="H184">
+        <v>0.245</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A185" t="s">
+        <v>22</v>
+      </c>
+      <c r="B185" t="s">
+        <v>4</v>
+      </c>
+      <c r="G185">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="H185">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A186" t="s">
+        <v>22</v>
+      </c>
+      <c r="B186" t="s">
+        <v>4</v>
+      </c>
+      <c r="G186">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="H186">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A187" t="s">
+        <v>22</v>
+      </c>
+      <c r="B187" t="s">
+        <v>4</v>
+      </c>
+      <c r="G187">
+        <v>0.19</v>
+      </c>
+      <c r="H187">
+        <v>0.19500000000000001</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A188" t="s">
+        <v>22</v>
+      </c>
+      <c r="B188" t="s">
+        <v>4</v>
+      </c>
+      <c r="G188">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="H188">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A189" t="s">
+        <v>22</v>
+      </c>
+      <c r="B189" t="s">
+        <v>4</v>
+      </c>
+      <c r="G189">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="H189">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A190" t="s">
+        <v>22</v>
+      </c>
+      <c r="B190" t="s">
+        <v>4</v>
+      </c>
+      <c r="G190">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="H190">
+        <v>0.35499999999999998</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A191" t="s">
+        <v>22</v>
+      </c>
+      <c r="B191" t="s">
+        <v>4</v>
+      </c>
+      <c r="G191">
+        <v>0.2</v>
+      </c>
+      <c r="H191">
+        <v>0.255</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A192" t="s">
+        <v>22</v>
+      </c>
+      <c r="B192" t="s">
+        <v>4</v>
+      </c>
+      <c r="G192">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="H192">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A193" t="s">
+        <v>22</v>
+      </c>
+      <c r="B193" t="s">
+        <v>4</v>
+      </c>
+      <c r="G193">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="H193">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A194" t="s">
+        <v>22</v>
+      </c>
+      <c r="B194" t="s">
+        <v>4</v>
+      </c>
+      <c r="G194">
+        <v>0.15</v>
+      </c>
+      <c r="H194">
+        <v>0.155</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A195" t="s">
+        <v>22</v>
+      </c>
+      <c r="B195" t="s">
+        <v>4</v>
+      </c>
+      <c r="G195">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H195">
+        <v>0.30499999999999999</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A196" t="s">
+        <v>22</v>
+      </c>
+      <c r="B196" t="s">
+        <v>4</v>
+      </c>
+      <c r="G196">
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="H196">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A197" t="s">
+        <v>22</v>
+      </c>
+      <c r="B197" t="s">
+        <v>4</v>
+      </c>
+      <c r="G197">
+        <v>0.45</v>
+      </c>
+      <c r="H197">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A198" t="s">
+        <v>22</v>
+      </c>
+      <c r="B198" t="s">
+        <v>4</v>
+      </c>
+      <c r="G198">
+        <v>0.11</v>
+      </c>
+      <c r="H198">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A199" t="s">
+        <v>22</v>
+      </c>
+      <c r="B199" t="s">
+        <v>4</v>
+      </c>
+      <c r="G199">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="H199">
+        <v>6.5000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A200" t="s">
+        <v>22</v>
+      </c>
+      <c r="B200" t="s">
+        <v>4</v>
+      </c>
+      <c r="G200">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H200">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A201" t="s">
+        <v>22</v>
+      </c>
+      <c r="B201" t="s">
+        <v>4</v>
+      </c>
+      <c r="G201">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="H201">
+        <v>0.245</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A202" t="s">
+        <v>22</v>
+      </c>
+      <c r="B202" t="s">
+        <v>4</v>
+      </c>
+      <c r="G202">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H202">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A203" t="s">
+        <v>22</v>
+      </c>
+      <c r="B203" t="s">
+        <v>4</v>
+      </c>
+      <c r="G203">
+        <v>0.08</v>
+      </c>
+      <c r="H203">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A204" t="s">
+        <v>22</v>
+      </c>
+      <c r="B204" t="s">
+        <v>4</v>
+      </c>
+      <c r="G204">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H204">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A205" t="s">
+        <v>22</v>
+      </c>
+      <c r="B205" t="s">
+        <v>4</v>
+      </c>
+      <c r="G205">
+        <v>0.52</v>
+      </c>
+      <c r="H205">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="206" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A206" t="s">
+        <v>22</v>
+      </c>
+      <c r="B206" t="s">
+        <v>4</v>
+      </c>
+      <c r="G206">
+        <v>0.24</v>
+      </c>
+      <c r="H206">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A207" t="s">
+        <v>22</v>
+      </c>
+      <c r="B207" t="s">
+        <v>4</v>
+      </c>
+      <c r="G207">
+        <v>0.23</v>
+      </c>
+      <c r="H207">
+        <v>0.245</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A208" t="s">
+        <v>22</v>
+      </c>
+      <c r="B208" t="s">
+        <v>4</v>
+      </c>
+      <c r="G208">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="H208">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A209" t="s">
+        <v>22</v>
+      </c>
+      <c r="B209" t="s">
+        <v>4</v>
+      </c>
+      <c r="G209">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="H209">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A210" t="s">
+        <v>22</v>
+      </c>
+      <c r="B210" t="s">
+        <v>4</v>
+      </c>
+      <c r="G210">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="H210">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="211" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A211" t="s">
+        <v>22</v>
+      </c>
+      <c r="B211" t="s">
+        <v>4</v>
+      </c>
+      <c r="G211">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="H211">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="212" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A212" t="s">
+        <v>22</v>
+      </c>
+      <c r="B212" t="s">
+        <v>4</v>
+      </c>
+      <c r="G212">
+        <v>0.17</v>
+      </c>
+      <c r="H212">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="213" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A213" t="s">
+        <v>22</v>
+      </c>
+      <c r="B213" t="s">
+        <v>4</v>
+      </c>
+      <c r="G213">
+        <v>0.34</v>
+      </c>
+      <c r="H213">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="214" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A214" t="s">
+        <v>22</v>
+      </c>
+      <c r="B214" t="s">
+        <v>4</v>
+      </c>
+      <c r="G214">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="H214">
+        <v>0.33</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1568,13 +4534,13 @@
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1585,7 +4551,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
@@ -1596,7 +4562,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
@@ -1607,7 +4573,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
@@ -1618,7 +4584,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
continued work on the rmd format
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MMAB3\Documents\RStudio Projects\Plant Nutrition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{464EA2DE-3E9B-42DA-8AB6-24920F53D2A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF4478C-0A9E-4390-A216-9307A37C8503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13845" yWindow="525" windowWidth="12540" windowHeight="14340" xr2:uid="{6DF183B6-C7A5-4299-88F5-06F25E78E8A8}"/>
+    <workbookView xWindow="1536" yWindow="600" windowWidth="12540" windowHeight="12360" xr2:uid="{6DF183B6-C7A5-4299-88F5-06F25E78E8A8}"/>
   </bookViews>
   <sheets>
     <sheet name="RFriendly" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="24">
   <si>
     <t>Species</t>
   </si>
@@ -53,9 +53,6 @@
   </si>
   <si>
     <t>Zero</t>
-  </si>
-  <si>
-    <t>Dalea</t>
   </si>
   <si>
     <t>A. fascicularis</t>
@@ -94,16 +91,22 @@
     <t>ShootDryWeight</t>
   </si>
   <si>
-    <t>Lespedeza</t>
+    <t>Lespedeza capitata</t>
   </si>
   <si>
-    <t>Asclepiastuberosa</t>
+    <t>Dalea candida</t>
   </si>
   <si>
-    <t>Amorpha</t>
+    <t>Asclepias tuberosa</t>
   </si>
   <si>
-    <t>Baptisia</t>
+    <t>Amorpha canescens</t>
+  </si>
+  <si>
+    <t>Baptisia bracteata</t>
+  </si>
+  <si>
+    <t>Asclepias incarnata</t>
   </si>
 </sst>
 </file>
@@ -512,11 +515,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0C02CD2-F61D-4638-82A2-24C13D55C41E}">
-  <dimension ref="A1:I214"/>
+  <dimension ref="A1:I300"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A160" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E210" sqref="E210"/>
+      <pane ySplit="1" topLeftCell="A270" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B284" sqref="B284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -539,27 +542,27 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -589,7 +592,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -619,7 +622,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -649,7 +652,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -679,7 +682,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
@@ -709,7 +712,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
@@ -739,7 +742,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
@@ -769,7 +772,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
@@ -799,7 +802,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
         <v>4</v>
@@ -829,7 +832,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
@@ -859,7 +862,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
@@ -889,7 +892,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
         <v>4</v>
@@ -919,7 +922,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
@@ -940,7 +943,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
@@ -961,7 +964,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
@@ -982,7 +985,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
@@ -1003,7 +1006,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
         <v>5</v>
@@ -1024,7 +1027,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>5</v>
@@ -1045,7 +1048,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>3</v>
@@ -1066,7 +1069,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
         <v>3</v>
@@ -1087,7 +1090,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
         <v>3</v>
@@ -1108,7 +1111,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B23" t="s">
         <v>3</v>
@@ -1129,7 +1132,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B24" t="s">
         <v>4</v>
@@ -1150,7 +1153,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B25" t="s">
         <v>4</v>
@@ -1171,7 +1174,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B26" t="s">
         <v>4</v>
@@ -1192,7 +1195,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B27" t="s">
         <v>4</v>
@@ -4519,6 +4522,1210 @@
       </c>
       <c r="H214">
         <v>0.33</v>
+      </c>
+    </row>
+    <row r="215" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A215" t="s">
+        <v>23</v>
+      </c>
+      <c r="B215" t="s">
+        <v>3</v>
+      </c>
+      <c r="G215">
+        <v>0.6</v>
+      </c>
+      <c r="H215">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A216" t="s">
+        <v>23</v>
+      </c>
+      <c r="B216" t="s">
+        <v>3</v>
+      </c>
+      <c r="G216">
+        <v>0.255</v>
+      </c>
+      <c r="H216">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="217" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A217" t="s">
+        <v>23</v>
+      </c>
+      <c r="B217" t="s">
+        <v>3</v>
+      </c>
+      <c r="G217">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="H217">
+        <v>0.77500000000000002</v>
+      </c>
+    </row>
+    <row r="218" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A218" t="s">
+        <v>23</v>
+      </c>
+      <c r="B218" t="s">
+        <v>3</v>
+      </c>
+      <c r="G218">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="H218">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="219" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A219" t="s">
+        <v>23</v>
+      </c>
+      <c r="B219" t="s">
+        <v>3</v>
+      </c>
+      <c r="G219">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="H219">
+        <v>0.53500000000000003</v>
+      </c>
+    </row>
+    <row r="220" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A220" t="s">
+        <v>23</v>
+      </c>
+      <c r="B220" t="s">
+        <v>3</v>
+      </c>
+      <c r="G220">
+        <v>0.36</v>
+      </c>
+      <c r="H220">
+        <v>0.42499999999999999</v>
+      </c>
+    </row>
+    <row r="221" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A221" t="s">
+        <v>23</v>
+      </c>
+      <c r="B221" t="s">
+        <v>3</v>
+      </c>
+      <c r="G221">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="H221">
+        <v>0.38500000000000001</v>
+      </c>
+    </row>
+    <row r="222" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A222" t="s">
+        <v>23</v>
+      </c>
+      <c r="B222" t="s">
+        <v>3</v>
+      </c>
+      <c r="G222">
+        <v>0.5</v>
+      </c>
+      <c r="H222">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="223" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A223" t="s">
+        <v>23</v>
+      </c>
+      <c r="B223" t="s">
+        <v>3</v>
+      </c>
+      <c r="G223">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="H223">
+        <v>0.47499999999999998</v>
+      </c>
+    </row>
+    <row r="224" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A224" t="s">
+        <v>23</v>
+      </c>
+      <c r="B224" t="s">
+        <v>3</v>
+      </c>
+      <c r="G224">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="H224">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="225" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A225" t="s">
+        <v>23</v>
+      </c>
+      <c r="B225" t="s">
+        <v>3</v>
+      </c>
+      <c r="G225">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="H225">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="226" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A226" t="s">
+        <v>23</v>
+      </c>
+      <c r="B226" t="s">
+        <v>3</v>
+      </c>
+      <c r="G226">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="H226">
+        <v>0.56499999999999995</v>
+      </c>
+    </row>
+    <row r="227" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A227" t="s">
+        <v>23</v>
+      </c>
+      <c r="B227" t="s">
+        <v>3</v>
+      </c>
+      <c r="G227">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="H227">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="228" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A228" t="s">
+        <v>23</v>
+      </c>
+      <c r="B228" t="s">
+        <v>3</v>
+      </c>
+      <c r="G228">
+        <v>0.4</v>
+      </c>
+      <c r="H228">
+        <v>0.30499999999999999</v>
+      </c>
+    </row>
+    <row r="229" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A229" t="s">
+        <v>23</v>
+      </c>
+      <c r="B229" t="s">
+        <v>3</v>
+      </c>
+      <c r="G229">
+        <v>0.45</v>
+      </c>
+      <c r="H229">
+        <v>0.36499999999999999</v>
+      </c>
+    </row>
+    <row r="230" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A230" t="s">
+        <v>23</v>
+      </c>
+      <c r="B230" t="s">
+        <v>3</v>
+      </c>
+      <c r="G230">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="H230">
+        <v>0.35499999999999998</v>
+      </c>
+    </row>
+    <row r="231" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A231" t="s">
+        <v>23</v>
+      </c>
+      <c r="B231" t="s">
+        <v>3</v>
+      </c>
+      <c r="G231">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="H231">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="232" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A232" t="s">
+        <v>23</v>
+      </c>
+      <c r="B232" t="s">
+        <v>3</v>
+      </c>
+      <c r="G232">
+        <v>0.43</v>
+      </c>
+      <c r="H232">
+        <v>0.26500000000000001</v>
+      </c>
+    </row>
+    <row r="233" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A233" t="s">
+        <v>23</v>
+      </c>
+      <c r="B233" t="s">
+        <v>3</v>
+      </c>
+      <c r="G233">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H233">
+        <v>0.36499999999999999</v>
+      </c>
+    </row>
+    <row r="234" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A234" t="s">
+        <v>23</v>
+      </c>
+      <c r="B234" t="s">
+        <v>3</v>
+      </c>
+      <c r="G234">
+        <v>0.35</v>
+      </c>
+      <c r="H234">
+        <v>0.36499999999999999</v>
+      </c>
+    </row>
+    <row r="235" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A235" t="s">
+        <v>23</v>
+      </c>
+      <c r="B235" t="s">
+        <v>3</v>
+      </c>
+      <c r="G235">
+        <v>0.32</v>
+      </c>
+      <c r="H235">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="236" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A236" t="s">
+        <v>23</v>
+      </c>
+      <c r="B236" t="s">
+        <v>3</v>
+      </c>
+      <c r="G236">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="H236">
+        <v>0.51500000000000001</v>
+      </c>
+    </row>
+    <row r="237" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A237" t="s">
+        <v>23</v>
+      </c>
+      <c r="B237" t="s">
+        <v>3</v>
+      </c>
+      <c r="G237">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="H237">
+        <v>0.57499999999999996</v>
+      </c>
+    </row>
+    <row r="238" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A238" t="s">
+        <v>23</v>
+      </c>
+      <c r="B238" t="s">
+        <v>3</v>
+      </c>
+      <c r="G238">
+        <v>0.4</v>
+      </c>
+      <c r="H238">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="239" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A239" t="s">
+        <v>23</v>
+      </c>
+      <c r="B239" t="s">
+        <v>3</v>
+      </c>
+      <c r="G239">
+        <v>0.72</v>
+      </c>
+      <c r="H239">
+        <v>0.73499999999999999</v>
+      </c>
+    </row>
+    <row r="240" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A240" t="s">
+        <v>23</v>
+      </c>
+      <c r="B240" t="s">
+        <v>3</v>
+      </c>
+      <c r="G240">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="H240">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="241" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A241" t="s">
+        <v>23</v>
+      </c>
+      <c r="B241" t="s">
+        <v>3</v>
+      </c>
+      <c r="G241">
+        <v>0.59</v>
+      </c>
+      <c r="H241">
+        <v>0.53500000000000003</v>
+      </c>
+    </row>
+    <row r="242" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A242" t="s">
+        <v>23</v>
+      </c>
+      <c r="B242" t="s">
+        <v>3</v>
+      </c>
+      <c r="G242">
+        <v>0.36</v>
+      </c>
+      <c r="H242">
+        <v>0.36499999999999999</v>
+      </c>
+    </row>
+    <row r="243" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A243" t="s">
+        <v>23</v>
+      </c>
+      <c r="B243" t="s">
+        <v>3</v>
+      </c>
+      <c r="G243">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="H243">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="244" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A244" t="s">
+        <v>23</v>
+      </c>
+      <c r="B244" t="s">
+        <v>3</v>
+      </c>
+      <c r="G244">
+        <v>0.35</v>
+      </c>
+      <c r="H244">
+        <v>0.55500000000000005</v>
+      </c>
+    </row>
+    <row r="245" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A245" t="s">
+        <v>23</v>
+      </c>
+      <c r="B245" t="s">
+        <v>3</v>
+      </c>
+      <c r="G245">
+        <v>0.34</v>
+      </c>
+      <c r="H245">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="246" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A246" t="s">
+        <v>23</v>
+      </c>
+      <c r="B246" t="s">
+        <v>3</v>
+      </c>
+      <c r="G246">
+        <v>0.31</v>
+      </c>
+      <c r="H246">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="247" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A247" t="s">
+        <v>23</v>
+      </c>
+      <c r="B247" t="s">
+        <v>3</v>
+      </c>
+      <c r="G247">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H247">
+        <v>0.33500000000000002</v>
+      </c>
+    </row>
+    <row r="248" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A248" t="s">
+        <v>23</v>
+      </c>
+      <c r="B248" t="s">
+        <v>3</v>
+      </c>
+      <c r="G248">
+        <v>0.64</v>
+      </c>
+      <c r="H248">
+        <v>0.91500000000000004</v>
+      </c>
+    </row>
+    <row r="249" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A249" t="s">
+        <v>23</v>
+      </c>
+      <c r="B249" t="s">
+        <v>3</v>
+      </c>
+      <c r="G249">
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="H249">
+        <v>0.51500000000000001</v>
+      </c>
+    </row>
+    <row r="250" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A250" t="s">
+        <v>23</v>
+      </c>
+      <c r="B250" t="s">
+        <v>3</v>
+      </c>
+      <c r="G250">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="H250">
+        <v>0.56499999999999995</v>
+      </c>
+    </row>
+    <row r="251" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A251" t="s">
+        <v>23</v>
+      </c>
+      <c r="B251" t="s">
+        <v>3</v>
+      </c>
+      <c r="G251">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="H251">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="252" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A252" t="s">
+        <v>23</v>
+      </c>
+      <c r="B252" t="s">
+        <v>3</v>
+      </c>
+      <c r="G252">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="H252">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="253" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A253" t="s">
+        <v>23</v>
+      </c>
+      <c r="B253" t="s">
+        <v>3</v>
+      </c>
+      <c r="G253">
+        <v>0.5</v>
+      </c>
+      <c r="H253">
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="254" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A254" t="s">
+        <v>23</v>
+      </c>
+      <c r="B254" t="s">
+        <v>3</v>
+      </c>
+      <c r="G254">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="H254">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="255" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A255" t="s">
+        <v>23</v>
+      </c>
+      <c r="B255" t="s">
+        <v>3</v>
+      </c>
+      <c r="G255">
+        <v>0.43</v>
+      </c>
+      <c r="H255">
+        <v>0.66500000000000004</v>
+      </c>
+    </row>
+    <row r="256" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A256" t="s">
+        <v>23</v>
+      </c>
+      <c r="B256" t="s">
+        <v>3</v>
+      </c>
+      <c r="G256">
+        <v>0.45</v>
+      </c>
+      <c r="H256">
+        <v>0.40500000000000003</v>
+      </c>
+    </row>
+    <row r="257" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A257" t="s">
+        <v>23</v>
+      </c>
+      <c r="B257" t="s">
+        <v>3</v>
+      </c>
+      <c r="G257">
+        <v>0.43</v>
+      </c>
+      <c r="H257">
+        <v>0.34499999999999997</v>
+      </c>
+    </row>
+    <row r="258" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A258" t="s">
+        <v>23</v>
+      </c>
+      <c r="B258" t="s">
+        <v>3</v>
+      </c>
+      <c r="G258">
+        <v>0.63</v>
+      </c>
+      <c r="H258">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="259" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A259" t="s">
+        <v>23</v>
+      </c>
+      <c r="B259" t="s">
+        <v>3</v>
+      </c>
+      <c r="G259">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="H259">
+        <v>0.47499999999999998</v>
+      </c>
+    </row>
+    <row r="260" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A260" t="s">
+        <v>23</v>
+      </c>
+      <c r="B260" t="s">
+        <v>3</v>
+      </c>
+      <c r="G260">
+        <v>0.15</v>
+      </c>
+      <c r="H260">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="261" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A261" t="s">
+        <v>23</v>
+      </c>
+      <c r="B261" t="s">
+        <v>3</v>
+      </c>
+      <c r="G261">
+        <v>0.48</v>
+      </c>
+      <c r="H261">
+        <v>0.52500000000000002</v>
+      </c>
+    </row>
+    <row r="262" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A262" t="s">
+        <v>23</v>
+      </c>
+      <c r="B262" t="s">
+        <v>3</v>
+      </c>
+      <c r="G262">
+        <v>0.375</v>
+      </c>
+      <c r="H262">
+        <v>0.35499999999999998</v>
+      </c>
+    </row>
+    <row r="263" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A263" t="s">
+        <v>23</v>
+      </c>
+      <c r="B263" t="s">
+        <v>3</v>
+      </c>
+      <c r="G263">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="H263">
+        <v>0.45500000000000002</v>
+      </c>
+    </row>
+    <row r="264" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A264" t="s">
+        <v>23</v>
+      </c>
+      <c r="B264" t="s">
+        <v>4</v>
+      </c>
+      <c r="G264">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="H264">
+        <v>0.44500000000000001</v>
+      </c>
+    </row>
+    <row r="265" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A265" t="s">
+        <v>23</v>
+      </c>
+      <c r="B265" t="s">
+        <v>4</v>
+      </c>
+      <c r="G265">
+        <v>0.5</v>
+      </c>
+      <c r="H265">
+        <v>0.84499999999999997</v>
+      </c>
+    </row>
+    <row r="266" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A266" t="s">
+        <v>23</v>
+      </c>
+      <c r="B266" t="s">
+        <v>4</v>
+      </c>
+      <c r="G266">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="H266">
+        <v>0.35499999999999998</v>
+      </c>
+    </row>
+    <row r="267" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A267" t="s">
+        <v>23</v>
+      </c>
+      <c r="B267" t="s">
+        <v>4</v>
+      </c>
+      <c r="G267">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H267">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="268" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A268" t="s">
+        <v>23</v>
+      </c>
+      <c r="B268" t="s">
+        <v>4</v>
+      </c>
+      <c r="G268">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="H268">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="269" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A269" t="s">
+        <v>23</v>
+      </c>
+      <c r="B269" t="s">
+        <v>4</v>
+      </c>
+      <c r="G269">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="H269">
+        <v>0.55500000000000005</v>
+      </c>
+    </row>
+    <row r="270" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A270" t="s">
+        <v>23</v>
+      </c>
+      <c r="B270" t="s">
+        <v>4</v>
+      </c>
+      <c r="G270">
+        <v>0.15</v>
+      </c>
+      <c r="H270">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="271" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A271" t="s">
+        <v>23</v>
+      </c>
+      <c r="B271" t="s">
+        <v>4</v>
+      </c>
+      <c r="G271">
+        <v>0.61</v>
+      </c>
+      <c r="H271">
+        <v>0.51500000000000001</v>
+      </c>
+    </row>
+    <row r="272" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A272" t="s">
+        <v>23</v>
+      </c>
+      <c r="B272" t="s">
+        <v>4</v>
+      </c>
+      <c r="G272">
+        <v>0.54</v>
+      </c>
+      <c r="H272">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="273" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A273" t="s">
+        <v>23</v>
+      </c>
+      <c r="B273" t="s">
+        <v>4</v>
+      </c>
+      <c r="G273">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="H273">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="274" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A274" t="s">
+        <v>23</v>
+      </c>
+      <c r="B274" t="s">
+        <v>4</v>
+      </c>
+      <c r="G274">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="H274">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="275" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A275" t="s">
+        <v>23</v>
+      </c>
+      <c r="B275" t="s">
+        <v>4</v>
+      </c>
+      <c r="G275">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="H275">
+        <v>0.41499999999999998</v>
+      </c>
+    </row>
+    <row r="276" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A276" t="s">
+        <v>23</v>
+      </c>
+      <c r="B276" t="s">
+        <v>4</v>
+      </c>
+      <c r="G276">
+        <v>0.25</v>
+      </c>
+      <c r="H276">
+        <v>0.46500000000000002</v>
+      </c>
+    </row>
+    <row r="277" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A277" t="s">
+        <v>23</v>
+      </c>
+      <c r="B277" t="s">
+        <v>4</v>
+      </c>
+      <c r="G277">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="H277">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="278" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A278" t="s">
+        <v>23</v>
+      </c>
+      <c r="B278" t="s">
+        <v>4</v>
+      </c>
+      <c r="G278">
+        <v>0.375</v>
+      </c>
+      <c r="H278">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="279" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A279" t="s">
+        <v>23</v>
+      </c>
+      <c r="B279" t="s">
+        <v>4</v>
+      </c>
+      <c r="G279">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="H279">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="280" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A280" t="s">
+        <v>23</v>
+      </c>
+      <c r="B280" t="s">
+        <v>4</v>
+      </c>
+      <c r="G280">
+        <v>0.26</v>
+      </c>
+      <c r="H280">
+        <v>0.54500000000000004</v>
+      </c>
+    </row>
+    <row r="281" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A281" t="s">
+        <v>23</v>
+      </c>
+      <c r="B281" t="s">
+        <v>4</v>
+      </c>
+      <c r="G281">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="H281">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="282" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A282" t="s">
+        <v>23</v>
+      </c>
+      <c r="B282" t="s">
+        <v>4</v>
+      </c>
+      <c r="G282">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H282">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="283" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A283" t="s">
+        <v>23</v>
+      </c>
+      <c r="B283" t="s">
+        <v>4</v>
+      </c>
+      <c r="G283">
+        <v>0.04</v>
+      </c>
+      <c r="H283">
+        <v>0.17499999999999999</v>
+      </c>
+    </row>
+    <row r="284" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A284" t="s">
+        <v>23</v>
+      </c>
+      <c r="B284" t="s">
+        <v>4</v>
+      </c>
+      <c r="G284">
+        <v>0.66</v>
+      </c>
+      <c r="H284">
+        <v>0.55500000000000005</v>
+      </c>
+    </row>
+    <row r="285" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A285" t="s">
+        <v>23</v>
+      </c>
+      <c r="B285" t="s">
+        <v>4</v>
+      </c>
+      <c r="G285">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="H285">
+        <v>0.66500000000000004</v>
+      </c>
+    </row>
+    <row r="286" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A286" t="s">
+        <v>23</v>
+      </c>
+      <c r="B286" t="s">
+        <v>4</v>
+      </c>
+      <c r="G286">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="H286">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="287" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A287" t="s">
+        <v>23</v>
+      </c>
+      <c r="B287" t="s">
+        <v>4</v>
+      </c>
+      <c r="G287">
+        <v>0.5</v>
+      </c>
+      <c r="H287">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="288" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A288" t="s">
+        <v>23</v>
+      </c>
+      <c r="B288" t="s">
+        <v>4</v>
+      </c>
+      <c r="G288">
+        <v>0.78</v>
+      </c>
+      <c r="H288">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="289" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A289" t="s">
+        <v>23</v>
+      </c>
+      <c r="B289" t="s">
+        <v>4</v>
+      </c>
+      <c r="G289">
+        <v>0.255</v>
+      </c>
+      <c r="H289">
+        <v>0.47499999999999998</v>
+      </c>
+    </row>
+    <row r="290" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A290" t="s">
+        <v>23</v>
+      </c>
+      <c r="B290" t="s">
+        <v>4</v>
+      </c>
+      <c r="G290">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="H290">
+        <v>0.53500000000000003</v>
+      </c>
+    </row>
+    <row r="291" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A291" t="s">
+        <v>23</v>
+      </c>
+      <c r="B291" t="s">
+        <v>4</v>
+      </c>
+      <c r="G291">
+        <v>0.62</v>
+      </c>
+      <c r="H291">
+        <v>1.0649999999999999</v>
+      </c>
+    </row>
+    <row r="292" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A292" t="s">
+        <v>23</v>
+      </c>
+      <c r="B292" t="s">
+        <v>4</v>
+      </c>
+      <c r="G292">
+        <v>0.13</v>
+      </c>
+      <c r="H292">
+        <v>0.28499999999999998</v>
+      </c>
+    </row>
+    <row r="293" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A293" t="s">
+        <v>23</v>
+      </c>
+      <c r="B293" t="s">
+        <v>4</v>
+      </c>
+      <c r="G293">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="H293">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="294" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A294" t="s">
+        <v>23</v>
+      </c>
+      <c r="B294" t="s">
+        <v>4</v>
+      </c>
+      <c r="G294">
+        <v>0.67</v>
+      </c>
+      <c r="H294">
+        <v>0.72499999999999998</v>
+      </c>
+    </row>
+    <row r="295" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A295" t="s">
+        <v>23</v>
+      </c>
+      <c r="B295" t="s">
+        <v>4</v>
+      </c>
+      <c r="G295">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="H295">
+        <v>0.44500000000000001</v>
+      </c>
+    </row>
+    <row r="296" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A296" t="s">
+        <v>23</v>
+      </c>
+      <c r="B296" t="s">
+        <v>4</v>
+      </c>
+      <c r="G296">
+        <v>0.64</v>
+      </c>
+      <c r="H296">
+        <v>0.59499999999999997</v>
+      </c>
+    </row>
+    <row r="297" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A297" t="s">
+        <v>23</v>
+      </c>
+      <c r="B297" t="s">
+        <v>4</v>
+      </c>
+      <c r="G297">
+        <v>0.5</v>
+      </c>
+      <c r="H297">
+        <v>0.48499999999999999</v>
+      </c>
+    </row>
+    <row r="298" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A298" t="s">
+        <v>23</v>
+      </c>
+      <c r="B298" t="s">
+        <v>4</v>
+      </c>
+      <c r="G298">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="H298">
+        <v>0.59499999999999997</v>
+      </c>
+    </row>
+    <row r="299" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A299" t="s">
+        <v>23</v>
+      </c>
+      <c r="B299" t="s">
+        <v>4</v>
+      </c>
+      <c r="G299">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="H299">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="300" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A300" t="s">
+        <v>23</v>
+      </c>
+      <c r="B300" t="s">
+        <v>4</v>
+      </c>
+      <c r="G300">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="H300">
+        <v>0.44500000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -4548,51 +5755,51 @@
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>